<commit_message>
rounded the data in Flight Times.xlsx
</commit_message>
<xml_diff>
--- a/Flight Times.xlsx
+++ b/Flight Times.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesista\Documents\NetBeansProjects\DisasterGO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -176,6 +176,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -211,6 +228,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -363,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,7 +411,7 @@
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -400,7 +434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -425,8 +459,36 @@
       <c r="H2" s="1">
         <v>8.6805555555555566E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <f>B2*24</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:P2" si="0">C2*24</f>
+        <v>1.75</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>1.8333333333333335</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>1.75</v>
+      </c>
+      <c r="N2">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333335</v>
+      </c>
+      <c r="O2">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="P2">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333335</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -451,8 +513,36 @@
       <c r="H3" s="1">
         <v>0.17361111111111113</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <f t="shared" ref="J3:J8" si="1">B3*24</f>
+        <v>1.75</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K8" si="2">C3*24</f>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L8" si="3">D3*24</f>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M8" si="4">E3*24</f>
+        <v>5.5</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N8" si="5">F3*24</f>
+        <v>4.916666666666667</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O8" si="6">G3*24</f>
+        <v>4.083333333333333</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P8" si="7">H3*24</f>
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -477,8 +567,36 @@
       <c r="H4" s="1">
         <v>0.11458333333333333</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>1.8333333333333335</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="4"/>
+        <v>1.25</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="5"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="6"/>
+        <v>3.75</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="7"/>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -503,8 +621,36 @@
       <c r="H5" s="1">
         <v>5.2083333333333336E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>1.75</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>5.5</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="3"/>
+        <v>1.25</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="5"/>
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="6"/>
+        <v>1.75</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="7"/>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -529,8 +675,36 @@
       <c r="H6" s="1">
         <v>6.25E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>2.0833333333333335</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>4.916666666666667</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="3"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="4"/>
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="6"/>
+        <v>3.916666666666667</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -555,8 +729,36 @@
       <c r="H7" s="1">
         <v>0.14583333333333334</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>4.083333333333333</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>3.75</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>1.75</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="5"/>
+        <v>3.916666666666667</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -579,6 +781,244 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>2.0833333333333335</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>2.75</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="4"/>
+        <v>1.25</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="5"/>
+        <v>1.5</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="6"/>
+        <v>3.5</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f>ROUND(J2*4, 0)/4</f>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ref="K10:P10" si="8">ROUND(K2*4, 0)/4</f>
+        <v>1.75</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="8"/>
+        <v>1.75</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="8"/>
+        <v>1.75</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <f t="shared" ref="J11:P11" si="9">ROUND(J3*4, 0)/4</f>
+        <v>1.75</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="9"/>
+        <v>4.25</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="9"/>
+        <v>5.5</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="9"/>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <f t="shared" ref="J12:P12" si="10">ROUND(J4*4, 0)/4</f>
+        <v>1.75</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="10"/>
+        <v>4.25</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="10"/>
+        <v>1.25</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="10"/>
+        <v>5.25</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="10"/>
+        <v>3.75</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="10"/>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <f t="shared" ref="J13:P13" si="11">ROUND(J5*4, 0)/4</f>
+        <v>1.75</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="11"/>
+        <v>5.5</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="11"/>
+        <v>1.25</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="11"/>
+        <v>1.75</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="11"/>
+        <v>1.75</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="11"/>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f t="shared" ref="J14:P14" si="12">ROUND(J6*4, 0)/4</f>
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="12"/>
+        <v>5.25</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="12"/>
+        <v>1.75</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="12"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <f t="shared" ref="J15:P15" si="13">ROUND(J7*4, 0)/4</f>
+        <v>1.5</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="13"/>
+        <v>3.75</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="13"/>
+        <v>1.75</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="13"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <f t="shared" ref="J16:P16" si="14">ROUND(J8*4, 0)/4</f>
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="14"/>
+        <v>4.25</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="14"/>
+        <v>2.75</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="14"/>
+        <v>1.25</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="14"/>
+        <v>1.5</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="14"/>
+        <v>3.5</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>